<commit_message>
Add Country code into db
</commit_message>
<xml_diff>
--- a/document/client_local_db.xlsx
+++ b/document/client_local_db.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="User Tab" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="139">
   <si>
     <t>Name</t>
   </si>
@@ -432,6 +432,18 @@
   </si>
   <si>
     <t>sequence id of the picture in this article, maximum is 9, same to webchat</t>
+  </si>
+  <si>
+    <t>senduserid</t>
+  </si>
+  <si>
+    <t>primary id in login user table</t>
+  </si>
+  <si>
+    <t>countrycode</t>
+  </si>
+  <si>
+    <t>country code</t>
   </si>
 </sst>
 </file>
@@ -546,7 +558,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -567,50 +579,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -708,18 +684,57 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:C20" totalsRowShown="0" headerRowDxfId="0" dataDxfId="7" headerRowBorderDxfId="1" tableBorderDxfId="6" totalsRowBorderDxfId="5">
-  <autoFilter ref="A4:C20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:C21" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+  <autoFilter ref="A4:C21"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Name" dataDxfId="4"/>
-    <tableColumn id="2" name="Type" dataDxfId="3"/>
-    <tableColumn id="3" name="Comments" dataDxfId="2"/>
+    <tableColumn id="1" name="Name" dataDxfId="2"/>
+    <tableColumn id="2" name="Type" dataDxfId="1"/>
+    <tableColumn id="3" name="Comments" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1010,10 +1025,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:C36"/>
+  <dimension ref="A3:C38"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1072,268 +1087,290 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="17" customFormat="1">
+      <c r="A9" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="B9" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:3">
+      <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="B10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:3" ht="30">
+      <c r="A11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C11" s="6" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" s="17" customFormat="1">
+      <c r="A14" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="2" t="s">
+      <c r="B14" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="1" t="s">
+    <row r="15" spans="1:3" s="17" customFormat="1">
+      <c r="A15" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="2" t="s">
+      <c r="B15" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B20" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
-      <c r="A20" s="3" t="s">
+    <row r="21" spans="1:3">
+      <c r="A21" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C21" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="7" t="s">
+    <row r="27" spans="1:3">
+      <c r="A27" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B27" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C27" s="7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" s="2"/>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>10</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C28" s="2"/>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" s="2" t="s">
+      <c r="B30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="30">
-      <c r="A30" s="2" t="s">
+    <row r="31" spans="1:3" ht="30">
+      <c r="A31" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B31" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C31" s="6" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" s="17" customFormat="1">
+      <c r="A34" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C33" s="2" t="s">
+      <c r="B34" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="2" t="s">
+    <row r="35" spans="1:3" s="17" customFormat="1">
+      <c r="A35" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C34" s="2" t="s">
+      <c r="B35" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="2" t="s">
+    <row r="36" spans="1:3" s="17" customFormat="1">
+      <c r="A36" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C35" s="2" t="s">
+      <c r="B37" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="2" t="s">
+    <row r="38" spans="1:3">
+      <c r="A38" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B38" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1348,10 +1385,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:C45"/>
+  <dimension ref="A2:C46"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1398,39 +1435,41 @@
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="8" t="s">
+      <c r="B7" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30">
-      <c r="A7" s="10" t="s">
+    <row r="8" spans="1:3" ht="30">
+      <c r="A8" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C8" s="11" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="8"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>4</v>
@@ -1439,201 +1478,201 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="8"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="8" t="s">
+      <c r="B11" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="12" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="14" customFormat="1">
-      <c r="A11" s="12" t="s">
+    <row r="12" spans="1:3" s="14" customFormat="1">
+      <c r="A12" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="12" t="s">
+      <c r="B12" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="B12" s="9"/>
     </row>
     <row r="13" spans="1:3">
       <c r="B13" s="9"/>
     </row>
     <row r="14" spans="1:3">
-      <c r="A14" t="s">
+      <c r="B14" s="9"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="7" t="s">
+    <row r="16" spans="1:3">
+      <c r="A16" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B16" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C16" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="2" t="s">
+    <row r="17" spans="1:3">
+      <c r="A17" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="2"/>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>42</v>
-      </c>
+      <c r="B17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>4</v>
+        <v>41</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>9</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>9</v>
+        <v>50</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C20" s="8"/>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
+      <c r="B21" s="8" t="s">
+        <v>4</v>
+      </c>
       <c r="C21" s="8"/>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="15"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="15"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="7" t="s">
+    <row r="26" spans="1:3">
+      <c r="A26" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B26" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C26" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="2" t="s">
+    <row r="27" spans="1:3">
+      <c r="A27" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C26" s="2"/>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="8" t="s">
+      <c r="B27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="2"/>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B27" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C27" s="8" t="s">
+      <c r="B28" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="10" t="s">
+    <row r="29" spans="1:3">
+      <c r="A29" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B28" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" s="8" t="s">
+      <c r="B29" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="8" t="s">
+    <row r="30" spans="1:3">
+      <c r="A30" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="B29" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" s="10" t="s">
+      <c r="B30" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" s="10" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="30">
-      <c r="A30" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="30">
       <c r="A31" s="8" t="s">
-        <v>57</v>
+        <v>5</v>
       </c>
       <c r="B31" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C31" s="11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="30">
+      <c r="A32" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="11" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C32" s="8"/>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="8" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B33" s="10" t="s">
         <v>4</v>
@@ -1642,103 +1681,112 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="8"/>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B34" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C34" s="8" t="s">
+      <c r="B35" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="8" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="14" customFormat="1">
-      <c r="A35" s="12" t="s">
+    <row r="36" spans="1:3" s="14" customFormat="1">
+      <c r="A36" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B35" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C35" s="12" t="s">
+      <c r="B36" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" s="12" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
-      <c r="A38" t="s">
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="7" t="s">
+    <row r="40" spans="1:3">
+      <c r="A40" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B40" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="C40" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="2" t="s">
+    <row r="41" spans="1:3">
+      <c r="A41" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C40" s="2"/>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="8" t="s">
+      <c r="B41" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" s="2"/>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B41" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C41" s="8" t="s">
+      <c r="B42" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="10" t="s">
+    <row r="43" spans="1:3">
+      <c r="A43" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B42" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C42" s="8" t="s">
+      <c r="B43" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="8" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="45">
-      <c r="A43" s="8" t="s">
+    <row r="44" spans="1:3" ht="45">
+      <c r="A44" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B43" s="10" t="s">
+      <c r="B44" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="C44" s="11" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C44" s="11" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C45" s="8"/>
+      <c r="B46" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C46" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1750,7 +1798,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A4:C25"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A20" sqref="A20:C25"/>
     </sheetView>
   </sheetViews>
@@ -1944,8 +1992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:C45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>